<commit_message>
Add acction 1 "Ingresar Placa"
</commit_message>
<xml_diff>
--- a/TestWorkShop1/TestWorkShop1/Default.xlsx
+++ b/TestWorkShop1/TestWorkShop1/Default.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Action1" sheetId="2" r:id="rId2"/>
+    <sheet name="IngresarPlaca" sheetId="2" r:id="rId2"/>
+    <sheet name="PagarMulta" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -473,10 +474,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="15.1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -486,7 +487,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -499,4 +500,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last Commit for Test Workshop
</commit_message>
<xml_diff>
--- a/TestWorkShop1/TestWorkShop1/Default.xlsx
+++ b/TestWorkShop1/TestWorkShop1/Default.xlsx
@@ -15,6 +15,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>device_manufacturer</t>
+  </si>
+  <si>
+    <t>Quito</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>CANTON</t>
+  </si>
+  <si>
+    <t>device_model</t>
+  </si>
+  <si>
+    <t>PCL-4426</t>
+  </si>
+  <si>
+    <t>Pichincha</t>
+  </si>
+  <si>
+    <t>device_ostype</t>
+  </si>
+  <si>
+    <t>Guayaquil</t>
+  </si>
+  <si>
+    <t>EDGE</t>
+  </si>
+  <si>
+    <t>PLACA</t>
+  </si>
+  <si>
+    <t>PROVINCIA</t>
+  </si>
+  <si>
+    <t>Guayas</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -155,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -163,15 +210,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,16 +568,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="7" width="9.41796875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1"/>
+    <row r="1" ht="14.95" s="5" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -491,12 +650,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -512,10 +671,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change chrome to firefox
</commit_message>
<xml_diff>
--- a/TestWorkShop1/TestWorkShop1/Default.xlsx
+++ b/TestWorkShop1/TestWorkShop1/Default.xlsx
@@ -27,13 +27,13 @@
     <t>Quito</t>
   </si>
   <si>
-    <t>CHROME</t>
-  </si>
-  <si>
     <t>CANTON</t>
   </si>
   <si>
     <t>device_model</t>
+  </si>
+  <si>
+    <t>FIREFOX</t>
   </si>
   <si>
     <t>PCL-4426</t>
@@ -235,9 +235,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -248,7 +246,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -267,11 +267,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -580,7 +580,7 @@
     <col min="8" max="16384" width="9.078125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="5" customFormat="1">
+    <row r="1" ht="14.95" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -588,18 +588,18 @@
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -631,11 +631,11 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>